<commit_message>
add new proyect oj java about matriz and random number and his exel table
</commit_message>
<xml_diff>
--- a/Trabajo de analisis.xlsx
+++ b/Trabajo de analisis.xlsx
@@ -5,27 +5,39 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC19\Desktop\perfectNumber\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC20\Desktop\perfectNumber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0E90A0-B4F4-4689-A22E-D1550815FCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971539F8-FCA3-4AAA-A028-3A374FF8ACBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{304ACAD7-2492-4B24-AB01-9B5FF1E8D717}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{304ACAD7-2492-4B24-AB01-9B5FF1E8D717}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Numero Perfecto" sheetId="1" r:id="rId1"/>
+    <sheet name="Matriz Random" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
   <si>
     <t>Valor</t>
   </si>
@@ -252,20 +264,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -298,7 +308,10 @@
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -386,7 +399,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$10</c:f>
+              <c:f>'Numero Perfecto'!$H$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -409,7 +422,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$11:$B$20</c:f>
+              <c:f>'Numero Perfecto'!$B$11:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -448,7 +461,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$11:$H$20</c:f>
+              <c:f>'Numero Perfecto'!$H$11:$H$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -753,7 +766,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$24</c:f>
+              <c:f>'Numero Perfecto'!$H$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -776,7 +789,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$25:$B$34</c:f>
+              <c:f>'Numero Perfecto'!$B$25:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -815,7 +828,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$25:$H$34</c:f>
+              <c:f>'Numero Perfecto'!$H$25:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1110,7 +1123,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$37</c:f>
+              <c:f>'Numero Perfecto'!$H$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1133,7 +1146,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$B$38:$B$47</c:f>
+              <c:f>'Numero Perfecto'!$B$38:$B$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1172,7 +1185,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$38:$H$47</c:f>
+              <c:f>'Numero Perfecto'!$H$38:$H$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1387,6 +1400,327 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Matriz Random'!$B$16:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Matriz Random'!$H$16:$H$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9509060</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13569060</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16057600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19509020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21382800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>517430260</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>518597360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1018358300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1024019560</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1535056080</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5C5-4E0D-AD5A-29A40E09DB1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1277162815"/>
+        <c:axId val="1277165215"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1277162815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1277165215"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1277165215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1277162815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1507,6 +1841,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2540,6 +2914,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3168,6 +4058,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A8C961-25AF-247D-517A-0533BF66FE91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4B7765F-7E73-4F3D-8A1E-E1F982B876D9}" name="Tabla1" displayName="Tabla1" ref="B10:H20" totalsRowShown="0">
   <autoFilter ref="B10:H20" xr:uid="{B4B7765F-7E73-4F3D-8A1E-E1F982B876D9}"/>
@@ -3181,7 +4112,7 @@
     <tableColumn id="4" xr3:uid="{B6762C6B-9BD9-43DE-9292-5A7945B5BD54}" name="T3"/>
     <tableColumn id="5" xr3:uid="{0CD3BDF0-33A0-4649-A9A8-B2480A440D39}" name="T4"/>
     <tableColumn id="6" xr3:uid="{41873EEF-7D12-4609-AB29-20815DFCB2AF}" name="T5"/>
-    <tableColumn id="7" xr3:uid="{5B8074DC-C11E-47A8-801C-40B5E4101C66}" name="Promedio" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{5B8074DC-C11E-47A8-801C-40B5E4101C66}" name="Promedio" dataDxfId="1">
       <calculatedColumnFormula>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3202,7 +4133,7 @@
     <tableColumn id="4" xr3:uid="{C979ECBD-A329-40DF-94A0-544224752C9E}" name="T3"/>
     <tableColumn id="5" xr3:uid="{9096A9F1-5850-42B2-ADA7-736FEB021A0E}" name="T4"/>
     <tableColumn id="6" xr3:uid="{5224EBA3-0570-482C-9C47-9711AF15B8B1}" name="T5"/>
-    <tableColumn id="7" xr3:uid="{C97D7035-CE6E-465E-984F-081E45491CFB}" name="Promedio" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{C97D7035-CE6E-465E-984F-081E45491CFB}" name="Promedio" dataDxfId="3">
       <calculatedColumnFormula>(Tabla13[[#This Row],[T1]]+Tabla13[[#This Row],[T2]]+Tabla13[[#This Row],[T3]]+Tabla13[[#This Row],[T4]]+Tabla13[[#This Row],[T5]])/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3223,8 +4154,29 @@
     <tableColumn id="4" xr3:uid="{8D9B1E73-F9E6-4FEB-9387-C49BF893EF2E}" name="T3"/>
     <tableColumn id="5" xr3:uid="{A6791223-ACC9-4EC1-9E2F-8264BA3D32B2}" name="T4"/>
     <tableColumn id="6" xr3:uid="{5D54CD2C-951C-4282-918B-17B7C1B9596C}" name="T5"/>
-    <tableColumn id="7" xr3:uid="{A4DB6DC6-C9D8-4776-9391-431CB43222FF}" name="Promedio" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{A4DB6DC6-C9D8-4776-9391-431CB43222FF}" name="Promedio" dataDxfId="2">
       <calculatedColumnFormula>(Tabla134[[#This Row],[T1]]+Tabla134[[#This Row],[T2]]+Tabla134[[#This Row],[T3]]+Tabla134[[#This Row],[T4]]+Tabla134[[#This Row],[T5]])/5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B0A6E83C-E9F5-4482-9761-F64467427E0D}" name="Tabla16" displayName="Tabla16" ref="B15:H25" totalsRowShown="0">
+  <autoFilter ref="B15:H25" xr:uid="{B0A6E83C-E9F5-4482-9761-F64467427E0D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B16:H25">
+    <sortCondition ref="B10:B20"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{EC4A9DDB-C77C-4B82-8798-195D6BD8EA26}" name="Valor"/>
+    <tableColumn id="2" xr3:uid="{D6CE568A-EE86-4D15-9B40-B0BBB7820619}" name="T1"/>
+    <tableColumn id="3" xr3:uid="{E3FA3D8C-93D7-4158-966B-E0E46DF53E43}" name="T2"/>
+    <tableColumn id="4" xr3:uid="{28556C54-FF36-44B6-911A-696176E45384}" name="T3"/>
+    <tableColumn id="5" xr3:uid="{199D987C-5E53-4721-B934-AF6F84FCEE59}" name="T4"/>
+    <tableColumn id="6" xr3:uid="{35D12DE6-B3ED-4A02-8F9D-7E226902A557}" name="T5"/>
+    <tableColumn id="7" xr3:uid="{D260D525-6FF5-4F6F-9B4A-AF812B568B55}" name="Promedio" dataDxfId="0">
+      <calculatedColumnFormula>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3530,8 +4482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1B845E-1BE4-4F60-B45B-737BD01267B9}">
   <dimension ref="B2:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3541,63 +4493,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -3623,25 +4575,25 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11">
         <v>200</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11">
         <v>200</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11">
         <v>300</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11">
         <v>300</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11">
         <v>200</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>240</v>
       </c>
@@ -3863,15 +4815,15 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -3897,25 +4849,25 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25">
         <v>188200</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25">
         <v>165700</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25">
         <v>175200</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25">
         <v>212000</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25">
         <v>182800</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25">
         <f>(Tabla13[[#This Row],[T1]]+Tabla13[[#This Row],[T2]]+Tabla13[[#This Row],[T3]]+Tabla13[[#This Row],[T4]]+Tabla13[[#This Row],[T5]])/5</f>
         <v>184780</v>
       </c>
@@ -4053,7 +5005,7 @@
       <c r="E31" s="1">
         <v>8570800</v>
       </c>
-      <c r="F31" s="4">
+      <c r="F31" s="3">
         <v>7686700</v>
       </c>
       <c r="G31" s="1">
@@ -4137,15 +5089,15 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -4171,25 +5123,25 @@
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="6">
+      <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38">
         <v>10370500</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38">
         <v>8480500</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38">
         <v>8092300</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38">
         <v>8334500</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38">
         <v>8165000</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38">
         <f>(Tabla134[[#This Row],[T1]]+Tabla134[[#This Row],[T2]]+Tabla134[[#This Row],[T3]]+Tabla134[[#This Row],[T4]]+Tabla134[[#This Row],[T5]])/5</f>
         <v>8688560</v>
       </c>
@@ -4285,7 +5237,7 @@
       <c r="F42">
         <v>8166200</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G42">
         <v>9422800</v>
       </c>
       <c r="H42">
@@ -4436,4 +5388,352 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68DA57F7-48AF-4B23-B57E-D3BA6CFD0748}">
+  <dimension ref="B5:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>9378800</v>
+      </c>
+      <c r="D16">
+        <v>9302800</v>
+      </c>
+      <c r="E16">
+        <v>8991300</v>
+      </c>
+      <c r="F16">
+        <v>9722000</v>
+      </c>
+      <c r="G16">
+        <v>10150400</v>
+      </c>
+      <c r="H16">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>9509060</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>12600100</v>
+      </c>
+      <c r="D17">
+        <v>13888600</v>
+      </c>
+      <c r="E17">
+        <v>13486400</v>
+      </c>
+      <c r="F17">
+        <v>14165800</v>
+      </c>
+      <c r="G17">
+        <v>13704400</v>
+      </c>
+      <c r="H17">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>13569060</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>15588000</v>
+      </c>
+      <c r="D18">
+        <v>16216500</v>
+      </c>
+      <c r="E18">
+        <v>16116400</v>
+      </c>
+      <c r="F18">
+        <v>16864400</v>
+      </c>
+      <c r="G18">
+        <v>15502700</v>
+      </c>
+      <c r="H18">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>16057600</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>18916000</v>
+      </c>
+      <c r="D19">
+        <v>19528100</v>
+      </c>
+      <c r="E19">
+        <v>19631400</v>
+      </c>
+      <c r="F19">
+        <v>19258500</v>
+      </c>
+      <c r="G19">
+        <v>20211100</v>
+      </c>
+      <c r="H19">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>19509020</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>21617300</v>
+      </c>
+      <c r="D20">
+        <v>21230500</v>
+      </c>
+      <c r="E20">
+        <v>21538700</v>
+      </c>
+      <c r="F20">
+        <v>21197500</v>
+      </c>
+      <c r="G20">
+        <v>21330000</v>
+      </c>
+      <c r="H20">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>21382800</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>60</v>
+      </c>
+      <c r="C21">
+        <v>514300800</v>
+      </c>
+      <c r="D21">
+        <v>519711600</v>
+      </c>
+      <c r="E21">
+        <v>515524000</v>
+      </c>
+      <c r="F21">
+        <v>521602000</v>
+      </c>
+      <c r="G21">
+        <v>516012900</v>
+      </c>
+      <c r="H21">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>517430260</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1">
+        <v>517665700</v>
+      </c>
+      <c r="D22" s="1">
+        <v>524917500</v>
+      </c>
+      <c r="E22" s="1">
+        <v>515846500</v>
+      </c>
+      <c r="F22" s="1">
+        <v>516681800</v>
+      </c>
+      <c r="G22" s="1">
+        <v>517875300</v>
+      </c>
+      <c r="H22" s="1">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>518597360</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>80</v>
+      </c>
+      <c r="C23">
+        <v>1014243800</v>
+      </c>
+      <c r="D23">
+        <v>1022730200</v>
+      </c>
+      <c r="E23">
+        <v>1016542400</v>
+      </c>
+      <c r="F23">
+        <v>1012842000</v>
+      </c>
+      <c r="G23">
+        <v>1025433100</v>
+      </c>
+      <c r="H23">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>1018358300</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>90</v>
+      </c>
+      <c r="C24">
+        <v>1024023000</v>
+      </c>
+      <c r="D24">
+        <v>1020915100</v>
+      </c>
+      <c r="E24">
+        <v>1028173100</v>
+      </c>
+      <c r="F24">
+        <v>1023269300</v>
+      </c>
+      <c r="G24">
+        <v>1023717300</v>
+      </c>
+      <c r="H24">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>1024019560</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>1530153100</v>
+      </c>
+      <c r="D25">
+        <v>1541613300</v>
+      </c>
+      <c r="E25">
+        <v>1539153800</v>
+      </c>
+      <c r="F25">
+        <v>1532147800</v>
+      </c>
+      <c r="G25">
+        <v>1532212400</v>
+      </c>
+      <c r="H25">
+        <f>(Tabla16[[#This Row],[T1]]+Tabla16[[#This Row],[T2]]+Tabla16[[#This Row],[T3]]+Tabla16[[#This Row],[T4]]+Tabla16[[#This Row],[T5]])/5</f>
+        <v>1535056080</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B5:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>